<commit_message>
Finish FASTA upload path
</commit_message>
<xml_diff>
--- a/public/seeding_template.xlsx
+++ b/public/seeding_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="180" windowWidth="21096" windowHeight="9612"/>
+    <workbookView xWindow="96" yWindow="180" windowWidth="21096" windowHeight="9612" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="7" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>NMIMR ID or NIHE_ID</t>
     <phoneticPr fontId="1"/>
@@ -428,14 +428,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CD4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>VL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>CD4計測日</t>
     <rPh sb="3" eb="5">
       <t>ケイソク</t>
@@ -534,6 +526,78 @@
       <t>スウジ</t>
     </rPh>
     <rPh sb="17" eb="19">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>serostatus</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>serostatus</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HIV-1/2血清学的状況</t>
+    <rPh sb="7" eb="9">
+      <t>ケッセイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ガク</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HIV-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HIV-2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dual</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unconfirmed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CD4: NDは0.1を、振り切れ値は9999を入力</t>
+    <rPh sb="13" eb="14">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VL: NDは0.1を、振り切れ値は999999999を入力</t>
+    <rPh sb="12" eb="13">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
       <t>ニュウリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -543,7 +607,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1519,13 +1583,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
@@ -1547,10 +1611,11 @@
     <col min="24" max="24" width="17.5546875" style="3" customWidth="1"/>
     <col min="25" max="25" width="12.6640625" customWidth="1"/>
     <col min="26" max="26" width="12.77734375" customWidth="1"/>
-    <col min="27" max="27" width="10.21875" customWidth="1"/>
+    <col min="27" max="27" width="12.77734375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="2" customFormat="1">
+    <row r="1" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1632,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
@@ -1591,22 +1656,22 @@
         <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>23</v>
@@ -1630,10 +1695,13 @@
         <v>20</v>
       </c>
       <c r="AA1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1644,7 +1712,7 @@
       <c r="L3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1673,7 +1741,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Instruction!$C$3:$C$6</xm:f>
@@ -1716,6 +1784,12 @@
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Instruction!$AA$3:$AA$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA1:AA1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1724,20 +1798,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="13" max="13" width="11.77734375" customWidth="1"/>
     <col min="18" max="19" width="8.88671875" style="1"/>
     <col min="20" max="20" width="11.21875" customWidth="1"/>
+    <col min="27" max="27" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +1829,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
@@ -1778,22 +1853,22 @@
         <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="T1" t="s">
         <v>22</v>
@@ -1816,11 +1891,14 @@
       <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="79.8" customHeight="1">
+    <row r="2" spans="1:28" ht="79.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1837,7 +1915,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>35</v>
@@ -1878,22 +1956,25 @@
         <v>67</v>
       </c>
       <c r="W2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>72</v>
-      </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>25</v>
       </c>
@@ -1913,10 +1994,13 @@
         <v>55</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>26</v>
       </c>
@@ -1936,10 +2020,13 @@
         <v>56</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -1958,8 +2045,11 @@
       <c r="L5" t="s">
         <v>57</v>
       </c>
+      <c r="AA5" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>28</v>
       </c>
@@ -1978,8 +2068,11 @@
       <c r="L6" t="s">
         <v>58</v>
       </c>
+      <c r="AA6" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I7" t="s">
         <v>41</v>
       </c>
@@ -1990,7 +2083,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
         <v>42</v>
       </c>
@@ -1998,7 +2091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I9" t="s">
         <v>43</v>
       </c>
@@ -2006,7 +2099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
         <v>44</v>
       </c>
@@ -2014,12 +2107,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>45</v>
       </c>

</xml_diff>